<commit_message>
Edited Halt pseudo instruction
</commit_message>
<xml_diff>
--- a/Reflex-8.xlsx
+++ b/Reflex-8.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\Code\dotnet_C#\R8_Compiler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\Code\dotnet_C#\R8_Assembler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72938F7-5EC1-4E18-AD49-6B717A2C9F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169E13A9-B9EC-4A2C-AE66-CB9DD6C0B4D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{521C1ACB-3572-404A-815D-1E6A034BF2CA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
   <si>
     <t>Fetch</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>Micro Code Instructions</t>
+  </si>
+  <si>
+    <t>Halt (pseudo instruction): Stops the clock. Determined by the most significant bit.</t>
   </si>
 </sst>
 </file>
@@ -378,16 +381,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -402,7 +400,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40 % - Accent3" xfId="1" builtinId="39"/>
@@ -722,7 +725,7 @@
   <dimension ref="A1:Y35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Y26" sqref="Y26"/>
+      <selection activeCell="Y23" sqref="Y23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -735,15 +738,15 @@
       <c r="A1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="15"/>
+      <c r="C1" s="22"/>
       <c r="D1" s="16"/>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="15"/>
+      <c r="F1" s="22"/>
       <c r="G1" s="16"/>
       <c r="H1" s="6" t="s">
         <v>23</v>
@@ -793,12 +796,12 @@
       <c r="W1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="Y1" s="22" t="s">
+      <c r="Y1" s="14" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -844,7 +847,7 @@
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A3" s="19"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="1"/>
       <c r="C3" s="9"/>
       <c r="D3" s="2"/>
@@ -882,7 +885,7 @@
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A4" s="19"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="1"/>
       <c r="C4" s="9"/>
       <c r="D4" s="2"/>
@@ -922,7 +925,7 @@
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A5" s="19"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="1"/>
       <c r="C5" s="9"/>
       <c r="D5" s="2"/>
@@ -960,7 +963,7 @@
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A6" s="20"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="3"/>
       <c r="C6" s="8"/>
       <c r="D6" s="5"/>
@@ -998,7 +1001,7 @@
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="20" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="1">
@@ -1042,7 +1045,7 @@
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="1"/>
       <c r="C8" s="9"/>
       <c r="D8" s="2"/>
@@ -1110,7 +1113,7 @@
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="15" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="1">
@@ -1158,7 +1161,7 @@
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="1"/>
       <c r="C11" s="9"/>
       <c r="D11" s="2"/>
@@ -1227,7 +1230,7 @@
       <c r="W12" s="10"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="1">
@@ -1270,12 +1273,12 @@
         <v>1</v>
       </c>
       <c r="W13" s="11"/>
-      <c r="Y13" s="22" t="s">
+      <c r="Y13" s="14" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="1"/>
       <c r="C14" s="9"/>
       <c r="D14" s="2"/>
@@ -1347,7 +1350,7 @@
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="1">
@@ -1395,7 +1398,7 @@
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="1"/>
       <c r="C17" s="9"/>
       <c r="D17" s="2"/>
@@ -1463,7 +1466,7 @@
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="1">
@@ -1511,7 +1514,7 @@
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="1"/>
       <c r="C20" s="9"/>
       <c r="D20" s="2"/>
@@ -1589,7 +1592,7 @@
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="1">
@@ -1636,7 +1639,7 @@
       <c r="W22" s="11"/>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
+      <c r="A23" s="15"/>
       <c r="B23" s="1"/>
       <c r="C23" s="9"/>
       <c r="D23" s="2"/>
@@ -1671,6 +1674,9 @@
       <c r="U23" s="9"/>
       <c r="V23" s="1"/>
       <c r="W23" s="11"/>
+      <c r="Y23" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
@@ -1712,7 +1718,7 @@
       <c r="W24" s="10"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="15" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="1">
@@ -1757,7 +1763,7 @@
       <c r="W25" s="11"/>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="1"/>
       <c r="C26" s="9"/>
       <c r="D26" s="2"/>
@@ -1819,7 +1825,7 @@
       <c r="W27" s="10"/>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="15" t="s">
         <v>29</v>
       </c>
       <c r="B28" s="1">
@@ -1860,7 +1866,7 @@
       <c r="W28" s="11"/>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A29" s="17"/>
+      <c r="A29" s="15"/>
       <c r="B29" s="1"/>
       <c r="C29" s="9"/>
       <c r="D29" s="2"/>
@@ -1922,7 +1928,7 @@
       <c r="W30" s="10"/>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="15" t="s">
         <v>28</v>
       </c>
       <c r="B31" s="1">
@@ -1965,7 +1971,7 @@
       <c r="W31" s="11"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A32" s="17"/>
+      <c r="A32" s="15"/>
       <c r="B32" s="1"/>
       <c r="C32" s="9"/>
       <c r="D32" s="2"/>
@@ -2062,6 +2068,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A28:A30"/>
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A9"/>
@@ -2069,11 +2080,6 @@
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A28:A30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>